<commit_message>
Change of graph, change of email sending(dynamic), change in reminding system, change in feeding logic
</commit_message>
<xml_diff>
--- a/consumption_data.xlsx
+++ b/consumption_data.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,78 +433,130 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Number of pellets</t>
+          <t>first feed number of pellets left</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>second feed number of pellets left</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total feed pellets fed</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>13 Nov</t>
+          <t>26 Nov</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>14 Nov</t>
+          <t>27 Nov</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="C3" t="n">
+        <v>42</v>
+      </c>
+      <c r="D3" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>15 Nov</t>
+          <t>28 Nov</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="C4" t="n">
+        <v>41</v>
+      </c>
+      <c r="D4" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>16 Nov</t>
+          <t>29 Nov</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>40</v>
+        <v>30</v>
+      </c>
+      <c r="C5" t="n">
+        <v>38</v>
+      </c>
+      <c r="D5" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>17 Nov</t>
+          <t>30 Nov</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="C6" t="n">
+        <v>35</v>
+      </c>
+      <c r="D6" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18 Nov</t>
+          <t>01 Dec</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="C7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D7" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>19 Nov</t>
+          <t>02 Dec</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C8" t="n">
+        <v>35</v>
+      </c>
+      <c r="D8" t="n">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>